<commit_message>
updated glossary allowed user to change password
</commit_message>
<xml_diff>
--- a/www/assets/templates/excel/weekly_report_glossary_template.xlsx
+++ b/www/assets/templates/excel/weekly_report_glossary_template.xlsx
@@ -11,14 +11,14 @@
   </sheets>
   <calcPr calcId="125725"/>
   <customWorkbookViews>
+    <customWorkbookView name="Rebecca Brasher - Personal View" guid="{D04B3ABB-E2E6-4A9B-A352-E51CECEAE162}" mergeInterval="0" personalView="1" maximized="1" xWindow="1" yWindow="1" windowWidth="1211" windowHeight="637" activeSheetId="1"/>
     <customWorkbookView name="cjohns - Personal View" guid="{5C5DCD9D-6124-4675-817B-7044BEA40FC4}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1911" windowHeight="883" activeSheetId="5"/>
-    <customWorkbookView name="Rebecca Brasher - Personal View" guid="{D04B3ABB-E2E6-4A9B-A352-E51CECEAE162}" mergeInterval="0" personalView="1" maximized="1" xWindow="1" yWindow="1" windowWidth="1211" windowHeight="637" activeSheetId="1"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="71">
   <si>
     <t>Middlebury Interactive Languages Report</t>
   </si>
@@ -75,12 +75,6 @@
   </si>
   <si>
     <t>Date student enrolled in the class.</t>
-  </si>
-  <si>
-    <t>Extra Credit Points</t>
-  </si>
-  <si>
-    <t>Extra credit points earned.</t>
   </si>
   <si>
     <t>Failing</t>
@@ -243,7 +237,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -268,10 +262,31 @@
     </font>
     <font>
       <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
       <i/>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -279,14 +294,8 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
-      <sz val="8"/>
+      <sz val="22"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -333,10 +342,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -355,20 +362,42 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -709,485 +738,482 @@
   <dimension ref="B2:D64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="27" customWidth="1"/>
-    <col min="3" max="3" width="54.140625" style="7" customWidth="1"/>
+    <col min="1" max="1" width="4.140625" customWidth="1"/>
+    <col min="2" max="2" width="27" style="5" customWidth="1"/>
+    <col min="3" max="3" width="78.140625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="3"/>
-      <c r="C2" s="4" t="s">
+    <row r="2" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B2" s="2"/>
+      <c r="C2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="3"/>
+      <c r="D2" s="1"/>
     </row>
     <row r="3" spans="2:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="3"/>
-      <c r="D3" s="3"/>
+      <c r="B3" s="2"/>
+      <c r="D3" s="1"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="8"/>
+      <c r="C6" s="6"/>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="8" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="9" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B11" s="11" t="s">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B13" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B14" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B15" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="12" t="s">
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B16" s="8" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
+      <c r="C16" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B20" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="B25" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="B26" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B27" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="B28" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B29" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B30" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B31" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+    </row>
+    <row r="33" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B33" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B34" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C34" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="1" t="s">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B35" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C35" s="8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B14" s="1" t="s">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B36" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="13" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C15" s="6" t="s">
+      <c r="C36" s="8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B37" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C37" s="8" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B16" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" s="6" t="s">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B38" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B39" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C39" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" s="6" t="s">
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B40" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B41" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C41" s="8" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="1" t="s">
+    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B42" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B43" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B44" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B45" s="4"/>
+      <c r="C45" s="7"/>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B46" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C46" s="17" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B47" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B48" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B49" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C49" s="8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B50" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B51" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C51" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B52" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C52" s="8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B53" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B19" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20" s="1" t="s">
+      <c r="C53" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B54" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C54" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B55" s="7"/>
+      <c r="C55" s="7"/>
+    </row>
+    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B56" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C56" s="17" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B57" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C57" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B58" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C58" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B59" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C59" s="8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B60" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C60" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B61" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C61" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B62" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B21" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B22" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B23" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" ht="45.75" x14ac:dyDescent="0.25">
-      <c r="B24" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3" ht="45.75" x14ac:dyDescent="0.25">
-      <c r="B25" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="26" spans="2:3" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B26" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="27" spans="2:3" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="B27" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B28" s="1" t="s">
+      <c r="C62" s="8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B63" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C63" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B64" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C28" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="29" spans="2:3" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B29" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="30" spans="2:3" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B30" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B31" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B32" s="1"/>
-      <c r="C32" s="6"/>
-    </row>
-    <row r="33" spans="2:3" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B33" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="C33" s="14" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B34" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B35" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B36" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C36" s="13" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B37" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C37" s="6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B38" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C38" s="6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="39" spans="2:3" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B39" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C39" s="6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B40" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C40" s="6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B41" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C41" s="6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B42" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C42" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B43" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C43" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B44" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C44" s="13" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B45" s="1"/>
-      <c r="C45" s="13"/>
-    </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B46" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="C46" s="13" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B47" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C47" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B48" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C48" s="13" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B49" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="C49" s="13" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B50" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="C50" s="13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="51" spans="2:3" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B51" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C51" s="13" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="52" spans="2:3" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B52" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="C52" s="13" t="s">
+      <c r="C64" s="8" t="s">
         <v>69</v>
-      </c>
-    </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B53" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C53" s="13" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B54" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="C54" s="13" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B55" s="16"/>
-      <c r="C55" s="13"/>
-    </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B56" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="C56" s="13" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B57" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C57" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B58" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C58" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B59" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="C59" s="13" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B60" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="C60" s="13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="61" spans="2:3" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B61" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C61" s="13" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="62" spans="2:3" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B62" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="C62" s="13" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B63" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C63" s="13" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B64" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="C64" s="13" t="s">
-        <v>71</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <customSheetViews>
-    <customSheetView guid="{5C5DCD9D-6124-4675-817B-7044BEA40FC4}">
+    <customSheetView guid="{D04B3ABB-E2E6-4A9B-A352-E51CECEAE162}">
       <selection activeCell="A9" sqref="A9:XFD9"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="landscape" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{D04B3ABB-E2E6-4A9B-A352-E51CECEAE162}">
+    <customSheetView guid="{5C5DCD9D-6124-4675-817B-7044BEA40FC4}">
       <selection activeCell="A9" sqref="A9:XFD9"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="landscape" r:id="rId2"/>

</xml_diff>